<commit_message>
Modified Excel for demo
</commit_message>
<xml_diff>
--- a/ProjectStatus.xlsx
+++ b/ProjectStatus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUNY-Buffalo\Course\Program\ProgrammingDataScience\GIT-Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\PythonRepos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF624135-23CB-452C-A801-3D5F772EE7A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B3449E-BE4F-4281-9356-26773F876E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{CD304F78-5A39-40EC-A1D6-CBD29B1BCCB9}"/>
   </bookViews>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t xml:space="preserve">Correlation of stock table and tweet table data </t>
-  </si>
-  <si>
-    <t>Interactive plots for represting sentiment analysis and its effects on stock data</t>
   </si>
   <si>
     <t xml:space="preserve">Project design document </t>
@@ -224,6 +221,9 @@
       </rPr>
       <t xml:space="preserve"> Finsihed coding for the preprocessing of tweet data and loading to database checked into Git                  </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactive plots for represting sentiment analysis and its effects on stock data </t>
   </si>
 </sst>
 </file>
@@ -936,7 +936,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -980,7 +980,7 @@
         <v>36</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="65" x14ac:dyDescent="0.35">
@@ -1029,7 +1029,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1040,7 +1040,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1051,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>

</xml_diff>

<commit_message>
Formatted and added new start file
</commit_message>
<xml_diff>
--- a/ProjectStatus.xlsx
+++ b/ProjectStatus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\PythonRepos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUNY-Buffalo\Course\Program\ProgrammingDataScience\GIT-Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B3449E-BE4F-4281-9356-26773F876E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA232298-7AE4-4266-842A-B35077AB62DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{CD304F78-5A39-40EC-A1D6-CBD29B1BCCB9}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Project</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">Interactive plots for represting sentiment analysis and its effects on stock data </t>
+  </si>
+  <si>
+    <t>05-04-Supreet - Formatted and uploaded into GIT - 05-09</t>
   </si>
 </sst>
 </file>
@@ -936,7 +939,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -994,9 +997,11 @@
         <v>38</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="16"/>
+        <v>36</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="6">

</xml_diff>